<commit_message>
default excel untuk mitra
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\project mitra\MitraBPS\ProjekMitraBPS\kito\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>nama</t>
   </si>
@@ -45,16 +45,39 @@
   </si>
   <si>
     <t>london enggress</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>tahun</t>
+  </si>
+  <si>
+    <t>email@gmail.com</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>+62 81</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,13 +100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,49 +389,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
template excel import survei
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -24,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>nama</t>
-  </si>
-  <si>
-    <t>alamat</t>
-  </si>
-  <si>
-    <t>desa</t>
-  </si>
-  <si>
-    <t>kecamatan</t>
-  </si>
-  <si>
-    <t>kelamin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>el fulano</t>
   </si>
@@ -47,19 +32,40 @@
     <t>london enggress</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>tahun</t>
   </si>
   <si>
     <t>email@gmail.com</t>
   </si>
   <si>
-    <t>hp</t>
-  </si>
-  <si>
     <t>+62 81</t>
+  </si>
+  <si>
+    <t>nama_lengkap</t>
+  </si>
+  <si>
+    <t>alamat_mitra</t>
+  </si>
+  <si>
+    <t>kode_desa</t>
+  </si>
+  <si>
+    <t>kode_kecamatan</t>
+  </si>
+  <si>
+    <t>jenis_kelamin</t>
+  </si>
+  <si>
+    <t>no_hp_mitra</t>
+  </si>
+  <si>
+    <t>email_mitra</t>
+  </si>
+  <si>
+    <t>kode_kabupaten</t>
+  </si>
+  <si>
+    <t>kode_provinsi</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -400,38 +406,44 @@
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -439,19 +451,19 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
template excel import mitra2survey
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -24,23 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>el fulano</t>
-  </si>
-  <si>
-    <t>london enggress</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>tahun</t>
   </si>
   <si>
-    <t>email@gmail.com</t>
-  </si>
-  <si>
-    <t>+62 81</t>
-  </si>
-  <si>
     <t>nama_lengkap</t>
   </si>
   <si>
@@ -66,6 +54,15 @@
   </si>
   <si>
     <t>kode_provinsi</t>
+  </si>
+  <si>
+    <t>contoh</t>
+  </si>
+  <si>
+    <t>contoh@gmail.com</t>
+  </si>
+  <si>
+    <t>+62 contoh</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -408,42 +405,42 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -455,10 +452,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menambahkan validasi untuk excel mitra dan memperbarui kolom excel
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\project mitra\MitraBPS\ProjekMitraBPS\kito\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIZKY\Documents\magang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CD6DD11-9C3E-4122-8AA7-F81337FADB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>tahun</t>
   </si>
@@ -62,13 +63,40 @@
     <t>contoh@gmail.com</t>
   </si>
   <si>
-    <t>+62 contoh</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>sobat_id</t>
+  </si>
+  <si>
+    <t>+62</t>
+  </si>
+  <si>
+    <t>16-02-2024</t>
+  </si>
+  <si>
+    <t>D001</t>
+  </si>
+  <si>
+    <t>KC001</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>1 = laki laki</t>
+  </si>
+  <si>
+    <t>2 = perempuan</t>
+  </si>
+  <si>
+    <t>1111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,10 +141,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -391,78 +426,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O3" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
menambah kondisi import mitra
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIZKY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8030F83D-52BD-4C0A-B706-20AC6EA3C7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD18208-AE2E-446E-9553-B5E80FB356F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E95CF797-8691-403B-8F70-13C90348AFEB}"/>
+    <workbookView xWindow="348" yWindow="948" windowWidth="15708" windowHeight="11088" xr2:uid="{E95CF797-8691-403B-8F70-13C90348AFEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>sobat_id</t>
   </si>
@@ -54,18 +54,12 @@
     <t>tahun</t>
   </si>
   <si>
-    <t>tahun_selesai</t>
-  </si>
-  <si>
     <t>D01</t>
   </si>
   <si>
     <t>KC1</t>
   </si>
   <si>
-    <t>1111</t>
-  </si>
-  <si>
     <t>contoh</t>
   </si>
   <si>
@@ -81,7 +75,13 @@
     <t>16-02-2024</t>
   </si>
   <si>
-    <t>16-03-2024</t>
+    <t>status_pekerjaan</t>
+  </si>
+  <si>
+    <t>detail_pekerjaan</t>
+  </si>
+  <si>
+    <t>1122</t>
   </si>
 </sst>
 </file>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F956DABC-A17B-4DD5-BB0A-4F7E51BAFDAA}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,7 +463,7 @@
     <col min="9" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,48 +483,54 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import seeder mitra dan tampilan edit survei
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIZKY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD18208-AE2E-446E-9553-B5E80FB356F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1444C5-AB4E-49E4-BA2B-FED55EE2F070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="948" windowWidth="15708" windowHeight="11088" xr2:uid="{E95CF797-8691-403B-8F70-13C90348AFEB}"/>
+    <workbookView xWindow="1920" yWindow="1872" windowWidth="15708" windowHeight="11088" xr2:uid="{E95CF797-8691-403B-8F70-13C90348AFEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>email_mitra</t>
   </si>
   <si>
-    <t>tahun</t>
-  </si>
-  <si>
     <t>D01</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>1122</t>
+  </si>
+  <si>
+    <t>tgl_mitra_diterima</t>
   </si>
 </sst>
 </file>
@@ -483,10 +483,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -495,42 +495,42 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
memperbarui excel dan kondisi status_pekerjaan mitra
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIZKY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1444C5-AB4E-49E4-BA2B-FED55EE2F070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D054F925-599D-41D5-B85C-B2055575185C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1872" windowWidth="15708" windowHeight="11088" xr2:uid="{E95CF797-8691-403B-8F70-13C90348AFEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E95CF797-8691-403B-8F70-13C90348AFEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +115,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,11 +138,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -153,6 +160,213 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455329A9-A67D-51C6-A914-706A8B2FD5E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="114300"/>
+          <a:ext cx="1752600" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1"/>
+            <a:t>(Boleh di isi boleh tidak)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="id-ID" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450" algn="l">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1"/>
+            <a:t>tgl_mitra_masuk</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+            <a:t> jika tidak di isi maka akan otomatis berisi tanggal saat ini</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-ID" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22165B83-0114-7772-DFA4-694A5DD318E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8633460" y="1463040"/>
+          <a:ext cx="1706880" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1"/>
+            <a:t>jenis_kelamin </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1"/>
+            <a:t>1 = laki-laki</a:t>
+          </a:r>
+          <a:endParaRPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+            <a:t>2 = perempuan</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+            <a:t>status_pekerjaan</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+            <a:t>0 = bisa mengikuti survei</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
+            <a:t>1 = tidak bisa mengikuti survei</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,7 +669,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,10 +693,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -494,7 +708,7 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -535,5 +749,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update template excel addmitra, perkondisian dan seeder
</commit_message>
<xml_diff>
--- a/kito/public/addMitra.xlsx
+++ b/kito/public/addMitra.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\project mitra\MitraBPS\ProjekMitraBPS\kito\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAE1313-FA4D-429F-8231-F5A4BC38CBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7180"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>sobat_id</t>
   </si>
@@ -53,15 +63,9 @@
     <t>contoh</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>contoh@gmail.com</t>
   </si>
   <si>
-    <t>status_pekerjaan</t>
-  </si>
-  <si>
     <t>detail_pekerjaan</t>
   </si>
   <si>
@@ -87,12 +91,21 @@
   </si>
   <si>
     <t>+628122233444</t>
+  </si>
+  <si>
+    <t>kode_kabupaten</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Pr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +200,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{455329A9-A67D-51C6-A914-706A8B2FD5E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455329A9-A67D-51C6-A914-706A8B2FD5E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -347,118 +360,6 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:endParaRPr lang="en-ID" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{22165B83-0114-7772-DFA4-694A5DD318E0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8641080" y="2148840"/>
-          <a:ext cx="1706880" cy="1638300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="171450" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1"/>
-            <a:t>jenis_kelamin </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1"/>
-            <a:t>1 = laki-laki</a:t>
-          </a:r>
-          <a:endParaRPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-            <a:t>2 = perempuan</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-            <a:t>status_pekerjaan</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-            <a:t>0 = bisa mengikuti survei</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-            <a:t>1 = tidak bisa mengikuti survei</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -763,21 +664,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" customWidth="1"/>
+    <col min="9" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,19 +689,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -809,15 +710,15 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -826,31 +727,31 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>